<commit_message>
new perfect doctor assignment
</commit_message>
<xml_diff>
--- a/Exercises/Perfect_Doctor.xlsx
+++ b/Exercises/Perfect_Doctor.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/Mixtape_tracks/Assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/git/Baylor-Causal-Inference/Exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673C66E6-8AA4-6B4D-95EB-BCF49F3E42BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946A2CC5-CD5A-5F49-BA8A-0DD3E0F53CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1060" windowWidth="24840" windowHeight="25820" activeTab="1" xr2:uid="{083BD555-0A53-1B4B-AE70-5F7A5361EDB7}"/>
+    <workbookView xWindow="940" yWindow="500" windowWidth="36800" windowHeight="21100" activeTab="3" xr2:uid="{083BD555-0A53-1B4B-AE70-5F7A5361EDB7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="together" sheetId="1" r:id="rId1"/>
+    <sheet name="in class" sheetId="2" r:id="rId2"/>
+    <sheet name="homework part a" sheetId="3" r:id="rId3"/>
+    <sheet name="homework part b" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="53">
   <si>
     <t>Person</t>
   </si>
@@ -120,6 +122,78 @@
   </si>
   <si>
     <t>Avg(Y |D=1) - Avg(Y |D=0)</t>
+  </si>
+  <si>
+    <t>TE = Y1-Y0 for each person</t>
+  </si>
+  <si>
+    <t>if TE&gt;0, the 'perfect dr.' assigns D=1 (vent)</t>
+  </si>
+  <si>
+    <t>If TE&lt;=0, he assigns no vent (D=0)</t>
+  </si>
+  <si>
+    <t>Y=DY1 + (1-D)Y0</t>
+  </si>
+  <si>
+    <t>The perfect dr knows whether the treatment helps or hurts, and</t>
+  </si>
+  <si>
+    <t>assigns the treatment based on whether it helps (TE&gt;0), or hurts (TE&lt;=0)</t>
+  </si>
+  <si>
+    <t>SDO = E[Y|D=1] - E[Y|D=0]</t>
+  </si>
+  <si>
+    <t>Comparing treatment to control, the people</t>
+  </si>
+  <si>
+    <t>on the vents' health is 1.34 units higher than</t>
+  </si>
+  <si>
+    <t>the people not on the vents.</t>
+  </si>
+  <si>
+    <t>"Decomposition of the SDO into its three parts"</t>
+  </si>
+  <si>
+    <t>Pi = E[D=1]</t>
+  </si>
+  <si>
+    <t>SDO = ATE + E[Y0|D=1] - E[Y0|D=0] + (1-pi)(ATT-ATU)</t>
+  </si>
+  <si>
+    <t>1. Calculate TE</t>
+  </si>
+  <si>
+    <t>3. Calculate the SDO</t>
+  </si>
+  <si>
+    <t>2. Perfect Doctor treatment assignment (D and Y)</t>
+  </si>
+  <si>
+    <t>4. Calculate</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>5. Decompose the SDO and show that it is equal to the formula</t>
+  </si>
+  <si>
+    <t>E[Y|D=1]</t>
+  </si>
+  <si>
+    <t>E[Y|D=0]</t>
+  </si>
+  <si>
+    <t>E[Y0|D=1]</t>
+  </si>
+  <si>
+    <t>E[Y0|D=0]</t>
+  </si>
+  <si>
+    <t>SDO DECOMPOSITION</t>
   </si>
 </sst>
 </file>
@@ -143,7 +217,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,8 +248,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -254,11 +334,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -275,6 +392,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,15 +711,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72EDE92-11F1-504D-AA85-77E1FD099BAB}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection sqref="A1:F13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,8 +741,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -634,12 +765,18 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="5">
         <f>E2*C2+(1-E2)*B2</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -656,12 +793,12 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="6">
         <f t="shared" ref="F3:F13" si="1">E3*C3+(1-E3)*B3</f>
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -678,12 +815,15 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -700,12 +840,12 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -722,12 +862,15 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -744,12 +887,15 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -766,12 +912,12 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -788,12 +934,18 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -810,12 +962,15 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -832,12 +987,15 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="6">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -854,12 +1012,12 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -876,12 +1034,12 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
@@ -889,14 +1047,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
-        <f>AVERAGE(F3,F5,F10:F11,F13) - AVERAGE(F2,F4,F6:F9,F12)</f>
+        <f>B17-C17</f>
         <v>1.3428571428571425</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f>AVERAGE(F13,F10:F11,F5,F3)</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C17">
+        <f>AVERAGE(F12,F6:F9,F4,F2)</f>
+        <v>6.8571428571428568</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>F20+A20-B20+(1-C20)*(D20-E20)</f>
+        <v>1.3428571428571425</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>19</v>
       </c>
@@ -916,49 +1087,67 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
-        <f>AVERAGE(B3,B5,B10:B11,B13)</f>
+        <f>AVERAGE(B3,B5,B10,B11,B13)</f>
         <v>3</v>
       </c>
       <c r="B20" s="13">
-        <f>AVERAGE(B2,B4,B6:B9,B12)</f>
+        <f>AVERAGE(B12,B9,B8,B7,B6,B4,B2)</f>
         <v>6.8571428571428568</v>
       </c>
       <c r="C20" s="12">
-        <f>SUM(E2:E13)/COUNT(E2:E13)</f>
+        <f>AVERAGE(E2:E13)</f>
         <v>0.41666666666666669</v>
       </c>
       <c r="D20" s="15">
-        <f>AVERAGE(D3,D5,D10:D11,D13)</f>
+        <f>AVERAGE(D3,D5,D10,D11,D13)</f>
         <v>5.2</v>
       </c>
       <c r="E20" s="13">
-        <f>AVERAGE(D2,D4,D6:D9,D12)</f>
+        <f>AVERAGE(D12,D9,D8,D7,D6,D4,D2)</f>
         <v>-3.2857142857142856</v>
       </c>
       <c r="F20" s="9">
         <f>AVERAGE(D2:D13)</f>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="H20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20">
+        <f>5/12</f>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <f>F20+ A20-B20+(1-C20)*(D20-E20)</f>
-        <v>1.3428571428571425</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -970,15 +1159,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658F0CAF-38BA-064D-B720-EB93DBD0638C}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -997,8 +1186,23 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1008,9 +1212,39 @@
       <c r="C2" s="6">
         <v>10</v>
       </c>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2" s="7">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>E2*C2+(1-E2)*B2</f>
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <f>G16-H16</f>
+        <v>-3.0285714285714285</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(E2:E13)</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(D2:D13)</f>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="J2">
+        <f>AVERAGE(D2:D3,D7,D9:D11,D13)</f>
+        <v>-2.4285714285714284</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE(D4:D6,D8,D12)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1020,9 +1254,19 @@
       <c r="C3" s="6">
         <v>15</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D13" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F13" si="1">E3*C3+(1-E3)*B3</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1032,9 +1276,23 @@
       <c r="C4" s="6">
         <v>12</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <f>I2+I16-J16+(1-H2)*(K2-J2)</f>
+        <v>-3.0285714285714294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1044,9 +1302,19 @@
       <c r="C5" s="6">
         <v>11</v>
       </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1056,9 +1324,19 @@
       <c r="C6" s="6">
         <v>9</v>
       </c>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1068,9 +1346,19 @@
       <c r="C7" s="6">
         <v>11</v>
       </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1080,9 +1368,19 @@
       <c r="C8" s="6">
         <v>7</v>
       </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1092,9 +1390,19 @@
       <c r="C9" s="6">
         <v>11</v>
       </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1104,9 +1412,19 @@
       <c r="C10" s="6">
         <v>6</v>
       </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1116,9 +1434,19 @@
       <c r="C11" s="6">
         <v>9</v>
       </c>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1128,9 +1456,19 @@
       <c r="C12" s="6">
         <v>13</v>
       </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1140,7 +1478,594 @@
       <c r="C13" s="6">
         <v>15</v>
       </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16">
+        <f>AVERAGE(F4:F6,F8,F12)</f>
+        <v>10.4</v>
+      </c>
+      <c r="H16">
+        <f>AVERAGE(F2:F3,F7,F9:F11,F13)</f>
+        <v>13.428571428571429</v>
+      </c>
+      <c r="I16">
+        <f>AVERAGE(B4:B6,B8,B12)</f>
+        <v>7.8</v>
+      </c>
+      <c r="J16">
+        <f>AVERAGE(B2:B3,B7,B9:B11,B13)</f>
+        <v>13.428571428571429</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0224CB-C32E-2849-913B-D3BC1D805D51}">
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5">
+        <v>80</v>
+      </c>
+      <c r="C2" s="6">
+        <v>81</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5">
+        <v>88</v>
+      </c>
+      <c r="C3" s="6">
+        <v>46</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5">
+        <v>68</v>
+      </c>
+      <c r="C4" s="6">
+        <v>33</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5">
+        <v>62</v>
+      </c>
+      <c r="C5" s="6">
+        <v>77</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="G5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5">
+        <v>71</v>
+      </c>
+      <c r="C6" s="6">
+        <v>83</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5">
+        <v>61</v>
+      </c>
+      <c r="C7" s="6">
+        <v>58</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5">
+        <v>100</v>
+      </c>
+      <c r="C8" s="6">
+        <v>34</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5">
+        <v>94</v>
+      </c>
+      <c r="C9" s="6">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="G9" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5">
+        <v>51</v>
+      </c>
+      <c r="C10" s="6">
+        <v>66</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="G10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5">
+        <v>93</v>
+      </c>
+      <c r="C11" s="6">
+        <v>57</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5">
+        <v>73</v>
+      </c>
+      <c r="C12" s="6">
+        <v>37</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="5">
+        <v>73</v>
+      </c>
+      <c r="C13" s="6">
+        <v>65</v>
+      </c>
       <c r="D13" s="7"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AACC999-4150-B944-BB59-31B4A186C121}">
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6">
+        <v>5</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="G5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6">
+        <v>13</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="G9" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5">
+        <v>13</v>
+      </c>
+      <c r="C10" s="6">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="G10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5">
+        <v>6</v>
+      </c>
+      <c r="C12" s="6">
+        <v>18</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="5">
+        <v>13</v>
+      </c>
+      <c r="C13" s="6">
+        <v>17</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>